<commit_message>
Login manager Req col
</commit_message>
<xml_diff>
--- a/docs/Login manager user story.xlsx
+++ b/docs/Login manager user story.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jolad\Documents\cse 3310\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimi\OneDrive\Documents\Courses\Fundamental of SWE\3310 Group project\cse3310_sp24_group_12\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A3D947C-ED1F-4FB9-B743-37D9E74AC9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB8D2A-771F-47D1-9847-6669AD7B7A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{85A1CE37-D265-4406-A8EF-DE321418B1E1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{85A1CE37-D265-4406-A8EF-DE321418B1E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,76 +36,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>EXPECTED OUTPUT</t>
-  </si>
-  <si>
-    <t>ACTUAL OUTPUT</t>
-  </si>
-  <si>
-    <t>first player enters site</t>
-  </si>
-  <si>
-    <t>player gets assigned as player_1 and is met with the login screen</t>
-  </si>
-  <si>
-    <t>player is met with log in screen upon entry</t>
-  </si>
-  <si>
-    <t>player_1 enters username "jimi"</t>
-  </si>
-  <si>
-    <t>Register prompt sent to loginimanager.registerUser, username is accepted and player is taken to Lobby</t>
-  </si>
-  <si>
-    <t>player is taken to lobby screen</t>
-  </si>
-  <si>
-    <t>second player enters site</t>
-  </si>
-  <si>
-    <t>player gets assigned as player_2 and is met with the login screen</t>
-  </si>
-  <si>
-    <t>player_2 enters username "jimi"</t>
-  </si>
-  <si>
-    <t>Register prompt sent to loginimanager.registerUser, "username already taken" displays for the player</t>
-  </si>
-  <si>
-    <t>"username already taken" error displays in red (login screen)</t>
-  </si>
-  <si>
-    <t>player_2 enters username "john"</t>
-  </si>
-  <si>
-    <t>third player enters site</t>
-  </si>
-  <si>
-    <t>player gets assigned as player_3 and is met with the login screen</t>
-  </si>
-  <si>
-    <t>player_3 eneters username "JO"</t>
-  </si>
-  <si>
-    <t>Register prompt sent to java, "Username must be at least 3 characters long" displays for the player</t>
-  </si>
-  <si>
-    <t>"Username must be at least 3 characters long" error is displayed in red (login screen)</t>
-  </si>
-  <si>
-    <t>player_3 eneters username "doe"</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Expected output</t>
+  </si>
+  <si>
+    <t>Actual Output</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Player 1 logs onto server</t>
+  </si>
+  <si>
+    <t>User should be prompted to enter nickname</t>
+  </si>
+  <si>
+    <t>User is prompted to enter nickname</t>
+  </si>
+  <si>
+    <t>SREQ002</t>
+  </si>
+  <si>
+    <t>Player 1 inputs "Player1" as nick</t>
+  </si>
+  <si>
+    <t>User should now be able to hit submit</t>
+  </si>
+  <si>
+    <t>User is able to hit submit</t>
+  </si>
+  <si>
+    <t>Player 1 hits submit</t>
+  </si>
+  <si>
+    <t>User should be taken to the game lobby and added to players list</t>
+  </si>
+  <si>
+    <t>SREQ004</t>
+  </si>
+  <si>
+    <t>Player 2 logs onto server</t>
+  </si>
+  <si>
+    <t>Player 2 inputs "Player2" as nick</t>
+  </si>
+  <si>
+    <t>Player 2 hits submit</t>
+  </si>
+  <si>
+    <t>Player 3 logs onto server</t>
+  </si>
+  <si>
+    <t>Player 3 inputs "Player3" as nick</t>
+  </si>
+  <si>
+    <t>Player 3 hits submit</t>
+  </si>
+  <si>
+    <t>Player 2 inputs "Player1" as nick</t>
+  </si>
+  <si>
+    <t>User should be given a "user already taken" error in red</t>
+  </si>
+  <si>
+    <t>User is given a "user already taken" error in red</t>
+  </si>
+  <si>
+    <t>Player 3 inputs "P3" as nick</t>
+  </si>
+  <si>
+    <t>SREQ003</t>
+  </si>
+  <si>
+    <t>User is taken to lobby and name is displayed on players list</t>
+  </si>
+  <si>
+    <t>User should be given a "Username must be at least 3 characters long" error in red</t>
+  </si>
+  <si>
+    <t>User is given a "Username must be at least 3 characters long" error in red</t>
+  </si>
+  <si>
+    <t>SREQ042</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,16 +139,28 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <i/>
+      <u/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,17 +179,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,120 +548,635 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5974E4-B7D5-4F84-8EC8-B1A7722F2664}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A4ABEE-EFFA-4B04-BAE6-84DCDBA8F38D}">
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="106.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75">
-      <c r="A3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="51">
+    <mergeCell ref="M27:P28"/>
+    <mergeCell ref="A25:D26"/>
+    <mergeCell ref="E25:H26"/>
+    <mergeCell ref="I25:L26"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="E27:H28"/>
+    <mergeCell ref="I27:L28"/>
+    <mergeCell ref="M23:P24"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="E15:H16"/>
+    <mergeCell ref="I15:L16"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="E17:H18"/>
+    <mergeCell ref="I17:L18"/>
+    <mergeCell ref="M17:P18"/>
+    <mergeCell ref="A21:D22"/>
+    <mergeCell ref="E21:H22"/>
+    <mergeCell ref="I21:L22"/>
+    <mergeCell ref="A23:D24"/>
+    <mergeCell ref="E23:H24"/>
+    <mergeCell ref="I23:L24"/>
+    <mergeCell ref="A13:D14"/>
+    <mergeCell ref="E13:H14"/>
+    <mergeCell ref="I13:L14"/>
+    <mergeCell ref="M13:P14"/>
+    <mergeCell ref="A19:D20"/>
+    <mergeCell ref="E19:H20"/>
+    <mergeCell ref="I19:L20"/>
+    <mergeCell ref="M19:P20"/>
+    <mergeCell ref="M7:P8"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="I9:L10"/>
+    <mergeCell ref="M9:P10"/>
+    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="E11:H12"/>
+    <mergeCell ref="I11:L12"/>
+    <mergeCell ref="A5:D6"/>
+    <mergeCell ref="E5:H6"/>
+    <mergeCell ref="I5:L6"/>
+    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="I1:L2"/>
+    <mergeCell ref="M1:P2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>